<commit_message>
Add many images from charts and scans. Also finish composing staff example
</commit_message>
<xml_diff>
--- a/_posts/_media_working_copies/IDesign/Staffing Charts.xlsx
+++ b/_posts/_media_working_copies/IDesign/Staffing Charts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\DevEssentialBlog\_posts\_media_working_copies\IDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBEA977-7A31-4424-A2F6-70D13B25145B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3325159-80B0-4698-AC9D-4229A3E1EFAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0744611-B43A-48DE-B010-E1CE23582270}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>Core staff</t>
   </si>
@@ -4539,6 +4538,617 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Reasonable</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core staff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$31:$M$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A6ED-474F-93BB-FC66CEF3FB5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core Staff 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$31:$N$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A6ED-474F-93BB-FC66CEF3FB5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Developer, etc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$31:$O$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A6ED-474F-93BB-FC66CEF3FB5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1297996671"/>
+        <c:axId val="1312544735"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1297996671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1312544735"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1312544735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1297996671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4819,6 +5429,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -7850,6 +8500,511 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8437,13 +9592,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8510,16 +9665,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8548,16 +9703,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8586,16 +9741,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8617,6 +9772,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19012380-12FF-4FD0-B5AC-6F49F9DA4F76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8925,7 +10118,7 @@
   <dimension ref="A1:X55"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30:K54"/>
+      <selection activeCell="M30" sqref="M30:O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10263,6 +11456,15 @@
       <c r="K30" t="s">
         <v>2</v>
       </c>
+      <c r="M30" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -10293,6 +11495,15 @@
         <f>5*(SIN(ROW())+2)</f>
         <v>7.9798117733846752</v>
       </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -10323,8 +11534,17 @@
         <f t="shared" ref="K32:K54" si="3">5*(SIN(ROW())+2)</f>
         <v>12.757133406208453</v>
       </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>2</v>
+      </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -10353,8 +11573,17 @@
         <f t="shared" si="3"/>
         <v>14.999559300536337</v>
       </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>2</v>
+      </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -10383,8 +11612,17 @@
         <f t="shared" si="3"/>
         <v>12.645413430600119</v>
       </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>4</v>
+      </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -10413,8 +11651,17 @@
         <f t="shared" si="3"/>
         <v>7.8590866525192453</v>
       </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>4</v>
+      </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -10443,8 +11690,17 @@
         <f t="shared" si="3"/>
         <v>5.0411057327844215</v>
       </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>4</v>
+      </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -10473,8 +11729,17 @@
         <f t="shared" si="3"/>
         <v>6.782309333215002</v>
       </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>4</v>
+      </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -10503,8 +11768,17 @@
         <f t="shared" si="3"/>
         <v>11.481842893546927</v>
       </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -10533,8 +11807,17 @@
         <f t="shared" si="3"/>
         <v>14.818976931420437</v>
       </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>6</v>
+      </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -10563,8 +11846,17 @@
         <f t="shared" si="3"/>
         <v>13.725565802396744</v>
       </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>6</v>
+      </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -10593,8 +11885,17 @@
         <f t="shared" si="3"/>
         <v>9.2068866559764544</v>
       </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>6</v>
+      </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -10623,8 +11924,17 @@
         <f t="shared" si="3"/>
         <v>5.4173922604218312</v>
       </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>6</v>
+      </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -10653,8 +11963,17 @@
         <f t="shared" si="3"/>
         <v>5.8411262868570084</v>
       </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>6</v>
+      </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -10683,8 +12002,17 @@
         <f t="shared" si="3"/>
         <v>10.088509625527069</v>
       </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44">
+        <v>6</v>
+      </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -10713,8 +12041,17 @@
         <f t="shared" si="3"/>
         <v>14.254517622670592</v>
       </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>6</v>
+      </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -10743,8 +12080,17 @@
         <f t="shared" si="3"/>
         <v>14.508941738244046</v>
       </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>6</v>
+      </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -10773,8 +12119,17 @@
         <f t="shared" si="3"/>
         <v>10.617865613726121</v>
       </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>4</v>
+      </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -10803,8 +12158,17 @@
         <f t="shared" si="3"/>
         <v>6.1587266933816665</v>
       </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>4</v>
+      </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -10833,8 +12197,17 @@
         <f t="shared" si="3"/>
         <v>5.2312367362026402</v>
       </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -10863,8 +12236,17 @@
         <f t="shared" si="3"/>
         <v>8.6881257314803566</v>
       </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -10893,8 +12275,17 @@
         <f t="shared" si="3"/>
         <v>13.351145879216872</v>
       </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51">
+        <v>2</v>
+      </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -10923,8 +12314,17 @@
         <f t="shared" si="3"/>
         <v>14.933137960202426</v>
       </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>2</v>
+      </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
@@ -10953,8 +12353,17 @@
         <f t="shared" si="3"/>
         <v>11.979625750909172</v>
       </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>2</v>
+      </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -10983,8 +12392,17 @@
         <f t="shared" si="3"/>
         <v>7.2060547557419188</v>
       </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>2</v>
+      </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
@@ -11004,8 +12422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0FC82A-56E5-4BB3-AB63-B9F70CF0C292}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>